<commit_message>
Deploying to gh-pages from @ Healthedata1/USCDI5-Sandbox@8fb17c3fd572c33cdd1fda0a4b0131db3cdef06b 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-us-core-interpreter-required.xlsx
+++ b/StructureDefinition-us-core-interpreter-required.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="118">
   <si>
     <t>Property</t>
   </si>
@@ -84,7 +84,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>This extension indicates that an interpreter to communicate healthcare information in the language specified in the extension's context. For example, if the extension is in the context of `Patient.communication.language` for Spanish, then an interpreter for Spanish is needed.</t>
+    <t>This extension indicates the individual's need for an interpreter to communicate healthcare information in a language other than the default language of the organization.</t>
   </si>
   <si>
     <t>Purpose</t>
@@ -135,13 +135,16 @@
     <t>Context</t>
   </si>
   <si>
-    <t>element:Patient.communication.language</t>
-  </si>
-  <si>
-    <t>element:RelatedPerson.communication.language</t>
-  </si>
-  <si>
-    <t>element:Practitioner.communication</t>
+    <t>element:Encounter</t>
+  </si>
+  <si>
+    <t>element:Patient</t>
+  </si>
+  <si>
+    <t>element:RelatedPerson</t>
+  </si>
+  <si>
+    <t>element:Practitioner</t>
   </si>
   <si>
     <t>ID</t>
@@ -271,7 +274,7 @@
     <t>Whether the individual needs an interpreter</t>
   </si>
   <si>
-    <t>This individual needs an interpreter to communicate healthcare information in the language specified in the extension's context.</t>
+    <t>This individual needs an interpreter to communicate healthcare information.</t>
   </si>
   <si>
     <t>The individual does not speak the default language of the organization, and hence requires an interpreter.</t>
@@ -352,7 +355,7 @@
     <t>Extension.value[x]</t>
   </si>
   <si>
-    <t xml:space="preserve">code
+    <t xml:space="preserve">Coding
 </t>
   </si>
   <si>
@@ -506,7 +509,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -702,6 +705,14 @@
       </c>
       <c r="B24" t="s" s="2">
         <v>42</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="B25" t="s" s="2">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -760,115 +771,115 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B1" t="s" s="1">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s" s="1">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AH1" t="s" s="1">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AI1" t="s" s="1">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AJ1" t="s" s="1">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AK1" t="s" s="1">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2">
@@ -880,514 +891,514 @@
       </c>
       <c r="C2" s="2"/>
       <c r="D2" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G2" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H2" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I2" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J2" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K2" t="s" s="2">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="L2" t="s" s="2">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="M2" t="s" s="2">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="N2" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="O2" s="2"/>
       <c r="P2" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="Q2" s="2"/>
       <c r="R2" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="S2" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="T2" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="U2" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="V2" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="W2" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="X2" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="Y2" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="Z2" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AA2" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AB2" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AC2" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AD2" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AE2" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AF2" t="s" s="2">
         <v>32</v>
       </c>
       <c r="AG2" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH2" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AI2" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AJ2" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AK2" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G3" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H3" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I3" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J3" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K3" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L3" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="M3" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="Q3" s="2"/>
       <c r="R3" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="S3" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="T3" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="U3" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="V3" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="W3" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="X3" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="Y3" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="Z3" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AA3" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AB3" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AC3" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AD3" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AE3" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AF3" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AG3" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH3" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AI3" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AJ3" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AK3" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G4" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H4" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I4" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J4" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K4" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="L4" t="s" s="2">
         <v>32</v>
       </c>
       <c r="M4" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="Q4" s="2"/>
       <c r="R4" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="S4" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="T4" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="U4" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="V4" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="W4" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="X4" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="Y4" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="Z4" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AA4" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AB4" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AC4" t="s" s="2">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AD4" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AE4" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AF4" t="s" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AG4" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH4" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AI4" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AJ4" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AK4" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H5" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I5" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="M5" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="N5" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="O5" s="2"/>
       <c r="P5" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="Q5" s="2"/>
       <c r="R5" t="s" s="2">
         <v>3</v>
       </c>
       <c r="S5" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="T5" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="U5" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="V5" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="W5" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="X5" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="Y5" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="Z5" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AA5" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AB5" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AC5" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AD5" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AE5" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AF5" t="s" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AG5" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AH5" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AI5" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AJ5" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AK5" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G6" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H6" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I6" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J6" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="M6" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="Q6" s="2"/>
       <c r="R6" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="S6" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="T6" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="U6" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="V6" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="W6" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="X6" t="s" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="Y6" t="s" s="2">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="Z6" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="AA6" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AB6" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AC6" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AD6" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AE6" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AF6" t="s" s="2">
+        <v>110</v>
+      </c>
+      <c r="AG6" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AH6" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="AI6" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AJ6" t="s" s="2">
+        <v>117</v>
+      </c>
+      <c r="AK6" t="s" s="2">
         <v>109</v>
-      </c>
-      <c r="AG6" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AH6" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AI6" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AJ6" t="s" s="2">
-        <v>116</v>
-      </c>
-      <c r="AK6" t="s" s="2">
-        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ Healthedata1/USCDI5-Sandbox@689c61a49e5cd0a3964048744366fa46a58030e0 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-us-core-interpreter-required.xlsx
+++ b/StructureDefinition-us-core-interpreter-required.xlsx
@@ -368,7 +368,7 @@
     <t>required</t>
   </si>
   <si>
-    <t>Yes|No|Unknown|Not Asked (Use Snomed CT values in final version to meet USCDI terminology requirement)</t>
+    <t>Yes|No|Unknown|Not Asked ☞☞☞ Use Snomed CT values in final version to meet USCDI terminology requirement</t>
   </si>
   <si>
     <t>http://terminology.hl7.org/ValueSet/yes-no-unknown-not-asked</t>
@@ -755,7 +755,7 @@
     <col min="22" max="22" width="17.65625" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="19.03515625" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="18.859375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="101.32421875" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="105.40625" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="59.046875" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="22.71875" customWidth="true" bestFit="true"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ Healthedata1/USCDI5-Sandbox@4c15cefa0250f2c64cd259ec671cfe5d86ea3512 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-us-core-interpreter-required.xlsx
+++ b/StructureDefinition-us-core-interpreter-required.xlsx
@@ -368,10 +368,10 @@
     <t>required</t>
   </si>
   <si>
-    <t>Yes|No|Unknown|Not Asked ☞☞☞ Use Snomed CT values in final version to meet USCDI terminology requirement</t>
-  </si>
-  <si>
-    <t>http://terminology.hl7.org/ValueSet/yes-no-unknown-not-asked</t>
+    <t>Answer Set with Yes No and Unknowns</t>
+  </si>
+  <si>
+    <t>http://cts.nlm.nih.gov/fhir/ValueSet/2.16.840.1.113762.1.4.1267.16</t>
   </si>
   <si>
     <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
@@ -755,8 +755,8 @@
     <col min="22" max="22" width="17.65625" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="19.03515625" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="18.859375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="105.40625" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="59.046875" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="36.8046875" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="63.01953125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="22.71875" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="42.03515625" customWidth="true" bestFit="true"/>

</xml_diff>